<commit_message>
Regenerated the solution's code coverage and code metrics reports.
</commit_message>
<xml_diff>
--- a/Docs/N3XeS.CSharp.Common Code Metrics.xlsx
+++ b/Docs/N3XeS.CSharp.Common Code Metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\N3XeS\Common\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A28191D4-C15F-4805-9FE4-CE3D80FC8F3D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5DB4883-75F1-4280-9840-836D60024B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="23520" windowWidth="30030" windowHeight="14355" xr2:uid="{CF2977FD-08C5-45B0-B875-304152B5AF02}"/>
+    <workbookView xWindow="2070" yWindow="22650" windowWidth="33630" windowHeight="19320" xr2:uid="{7D40027E-F3F3-458A-A872-F255FC121C08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -66,7 +68,7 @@
     <t>Lines of Code</t>
   </si>
   <si>
-    <t>Source\N3XeS.CSharp.Common (Debug)</t>
+    <t>Source\N3XeS.CSharp.Common (Release)</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -438,18 +440,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA790EF-6FDC-44EA-84D7-73EA2D59180D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C134C5-5D72-46F2-907B-EEEFDFF2EAE9}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
@@ -506,19 +510,19 @@
         <v>11</v>
       </c>
       <c r="F2">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>141</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -538,7 +542,7 @@
         <v>11</v>
       </c>
       <c r="F3">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -547,10 +551,10 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -570,7 +574,7 @@
         <v>11</v>
       </c>
       <c r="F4">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -579,10 +583,10 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -602,16 +606,16 @@
         <v>14</v>
       </c>
       <c r="F5">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -631,19 +635,19 @@
         <v>11</v>
       </c>
       <c r="F6">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>3</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
       <c r="J6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -663,19 +667,19 @@
         <v>11</v>
       </c>
       <c r="F7">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
       <c r="J7">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -695,20 +699,20 @@
         <v>17</v>
       </c>
       <c r="F8">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="I8">
         <v>3</v>
       </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
       <c r="J8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J8" xr:uid="{4A8B4CA1-4F6B-4FC4-A081-1EB73C7F2ECA}"/>
+  <autoFilter ref="A1:J8" xr:uid="{F6D72773-3484-4239-9D28-69C48A6B0099}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added ReadOnlyException. Updated documentation, and regenerated reports.
</commit_message>
<xml_diff>
--- a/Docs/N3XeS.CSharp.Common Code Metrics.xlsx
+++ b/Docs/N3XeS.CSharp.Common Code Metrics.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\N3XeS\Common\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5DB4883-75F1-4280-9840-836D60024B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BFF5C7E-EEB8-4D6B-8E9C-113E4926B17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="22650" windowWidth="33630" windowHeight="19320" xr2:uid="{7D40027E-F3F3-458A-A872-F255FC121C08}"/>
+    <workbookView xWindow="1845" yWindow="22245" windowWidth="33630" windowHeight="19320" xr2:uid="{A267717C-209E-482E-9D41-5DE38B329B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="24">
   <si>
     <t>Scope</t>
   </si>
@@ -72,6 +72,24 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>N3XeS.CSharp.Common.Exceptions</t>
+  </si>
+  <si>
+    <t>ReadOnlyException</t>
+  </si>
+  <si>
+    <t>ReadOnlyException()</t>
+  </si>
+  <si>
+    <t>ReadOnlyException(SerializationInfo, StreamingContext)</t>
+  </si>
+  <si>
+    <t>ReadOnlyException(string)</t>
+  </si>
+  <si>
+    <t>ReadOnlyException(string, Exception)</t>
   </si>
   <si>
     <t>N3XeS.CSharp.Common.Extensions</t>
@@ -440,20 +458,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C134C5-5D72-46F2-907B-EEEFDFF2EAE9}">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF109CC1-C5B7-4DE5-8214-2F52220D6485}">
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
@@ -513,16 +531,16 @@
         <v>97</v>
       </c>
       <c r="G2">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J2">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -542,19 +560,19 @@
         <v>11</v>
       </c>
       <c r="F3">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -574,19 +592,19 @@
         <v>11</v>
       </c>
       <c r="F4">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -606,13 +624,13 @@
         <v>14</v>
       </c>
       <c r="F5">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -620,66 +638,60 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
       <c r="F6">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
       <c r="F7">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -690,29 +702,215 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
       <c r="F8">
+        <v>95</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>92</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>92</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>92</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
         <v>74</v>
       </c>
-      <c r="G8">
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="J8">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>74</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14">
+        <v>74</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J8" xr:uid="{F6D72773-3484-4239-9D28-69C48A6B0099}"/>
+  <autoFilter ref="A1:J14" xr:uid="{1C077D8E-7818-4297-9AF0-B54FD412149F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>